<commit_message>
fix driver for edge
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\MapScrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6366A60E-150E-4172-8AA5-AA8F7494E50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7152B64-5C13-461D-9897-F20B533844AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4ADDCA93-164A-410F-89B0-789B0CD35122}"/>
   </bookViews>
@@ -36,15 +36,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>bãi đỗ xe</t>
-  </si>
-  <si>
-    <t>bãi gửi xe</t>
-  </si>
-  <si>
-    <t>điểm trông xe</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>cà phê</t>
+  </si>
+  <si>
+    <t>cf</t>
+  </si>
+  <si>
+    <t>trà</t>
+  </si>
+  <si>
+    <t>cà phê sách</t>
+  </si>
+  <si>
+    <t>quán ăn</t>
+  </si>
+  <si>
+    <t>nhà hàng</t>
+  </si>
+  <si>
+    <t>sushi</t>
   </si>
 </sst>
 </file>
@@ -416,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C64AA0D-8A4A-44A9-BE02-F03A1FF64A3C}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +451,26 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixing get_attribute return None
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\MapScrapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Learning\Code\MapScrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7152B64-5C13-461D-9897-F20B533844AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183EE191-2BB6-4490-AAB0-C063A3A37E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{4ADDCA93-164A-410F-89B0-789B0CD35122}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28650" windowHeight="15345" xr2:uid="{4ADDCA93-164A-410F-89B0-789B0CD35122}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>cà phê</t>
-  </si>
-  <si>
-    <t>cf</t>
-  </si>
-  <si>
-    <t>trà</t>
-  </si>
-  <si>
-    <t>cà phê sách</t>
-  </si>
-  <si>
-    <t>quán ăn</t>
-  </si>
-  <si>
-    <t>nhà hàng</t>
-  </si>
-  <si>
-    <t>sushi</t>
   </si>
 </sst>
 </file>
@@ -67,7 +49,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -428,47 +410,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C64AA0D-8A4A-44A9-BE02-F03A1FF64A3C}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>